<commit_message>
first draft of script to amalgamate photos
</commit_message>
<xml_diff>
--- a/data/priorities.xlsx
+++ b/data/priorities.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\allan\OneDrive\New_Graph\Current\2019-023_Bulkley_fish_passage\scripts\Bulkley_Planning\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B786710-6AAE-4B4C-ABE4-AC6892445F91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B166FC24-3920-4FBC-942F-88BCFCB5268C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{821C12C4-A1B8-974C-A56E-63CAEF8E23F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,32 +33,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="66">
   <si>
     <t>hab_value</t>
   </si>
   <si>
-    <t>site_id</t>
-  </si>
-  <si>
     <t>priority</t>
   </si>
   <si>
     <t>comments</t>
   </si>
   <si>
-    <t>length</t>
-  </si>
-  <si>
     <t>length_of_new_habitat</t>
   </si>
   <si>
     <t>gazetted_names</t>
   </si>
   <si>
-    <t>Unnamed tributary to Blunt creek</t>
-  </si>
-  <si>
     <t>123794_ds</t>
   </si>
   <si>
@@ -161,18 +152,12 @@
     <t>1805608_ds</t>
   </si>
   <si>
-    <t>180608_us</t>
-  </si>
-  <si>
     <t>3042_us</t>
   </si>
   <si>
     <t>3042_ds</t>
   </si>
   <si>
-    <t xml:space="preserve">Tributary to McQuarrie Creek </t>
-  </si>
-  <si>
     <t>3139_ds</t>
   </si>
   <si>
@@ -194,9 +179,6 @@
     <t>1800213_ds</t>
   </si>
   <si>
-    <t xml:space="preserve">McDowell Creek </t>
-  </si>
-  <si>
     <t>58159_ds</t>
   </si>
   <si>
@@ -212,16 +194,43 @@
     <t>195290_us</t>
   </si>
   <si>
-    <t>125288_ds</t>
-  </si>
-  <si>
     <t>Riddeck Creek</t>
   </si>
   <si>
     <t>197360_ds</t>
   </si>
   <si>
-    <t>194360_us</t>
+    <t>124504_us</t>
+  </si>
+  <si>
+    <t>Tributary to McQuarrie Creek</t>
+  </si>
+  <si>
+    <t>McDowell Creek</t>
+  </si>
+  <si>
+    <t>195288_ds</t>
+  </si>
+  <si>
+    <t>197360_us</t>
+  </si>
+  <si>
+    <t>electrofishing</t>
+  </si>
+  <si>
+    <t>minnowtrapping</t>
+  </si>
+  <si>
+    <t>uav_survey</t>
+  </si>
+  <si>
+    <t>survey_length_m</t>
+  </si>
+  <si>
+    <t>local_name</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -573,371 +582,569 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A10DE3F-E4A8-B34E-806F-E8347038A62A}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>525</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>650</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C9">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C10">
+        <v>1400</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C11">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C12">
+        <v>300</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C13">
+        <v>1200</v>
+      </c>
+      <c r="E13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C14">
+        <v>300</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C15">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C16">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C18">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="C19">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" t="s">
         <v>30</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C21">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C22">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>34</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C23">
+        <v>520</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C24">
+        <v>450</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C25">
+        <v>300</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>37</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26">
+        <v>415</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C27">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" t="s">
         <v>40</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C28">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="C29">
+        <v>285</v>
+      </c>
+      <c r="D29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="C30">
+        <v>625</v>
+      </c>
+      <c r="D30" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C31">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
         <v>45</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C32">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="C33">
+        <v>690</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="C34">
+        <v>300</v>
+      </c>
+      <c r="D34" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" t="s">
         <v>48</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C35">
+        <v>135</v>
+      </c>
+      <c r="D35" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="C36">
+        <v>440</v>
+      </c>
+      <c r="D36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="C37">
+        <v>150</v>
+      </c>
+      <c r="D37" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C38">
+        <v>150</v>
+      </c>
+      <c r="D38" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>50</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39">
+        <v>250</v>
+      </c>
+      <c r="F39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>53</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B40" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="C40">
+        <v>300</v>
+      </c>
+      <c r="D40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>53</v>
       </c>
-      <c r="B36" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>56</v>
-      </c>
-      <c r="B37" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>56</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" t="s">
-        <v>62</v>
+      <c r="C41">
+        <v>1200</v>
+      </c>
+      <c r="D41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>